<commit_message>
change image of arrow and add some Anvil ships
</commit_message>
<xml_diff>
--- a/ANVIL/ANVIL ship list.xlsx
+++ b/ANVIL/ANVIL ship list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Git\ship-render\ANVIL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57B0B81-C26D-4A42-BE95-7ACADCB36240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDCC25E-30AF-4988-989E-A5D21D4D1898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13350" yWindow="3375" windowWidth="13545" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>船名（中文）</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -571,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -763,6 +763,9 @@
       <c r="D11">
         <v>1</v>
       </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -777,6 +780,9 @@
       <c r="D12">
         <v>1</v>
       </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -805,6 +811,12 @@
       <c r="C14">
         <v>175</v>
       </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -816,6 +828,12 @@
       <c r="C15">
         <v>180</v>
       </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -827,6 +845,12 @@
       <c r="C16">
         <v>195</v>
       </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -838,6 +862,12 @@
       <c r="C17">
         <v>195</v>
       </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -849,6 +879,9 @@
       <c r="C18">
         <v>220</v>
       </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -860,6 +893,9 @@
       <c r="C19">
         <v>350</v>
       </c>
+      <c r="F19" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
@@ -871,6 +907,9 @@
       <c r="C20">
         <v>375</v>
       </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -882,6 +921,9 @@
       <c r="C21">
         <v>375</v>
       </c>
+      <c r="F21" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -892,6 +934,9 @@
       </c>
       <c r="C22">
         <v>575</v>
+      </c>
+      <c r="F22" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Only Carrack Leftgit add ANVIL/*!
</commit_message>
<xml_diff>
--- a/ANVIL/ANVIL ship list.xlsx
+++ b/ANVIL/ANVIL ship list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Git\ship-render\ANVIL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDCC25E-30AF-4988-989E-A5D21D4D1898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA4F65A-79B5-4E3F-904E-61911414683E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13350" yWindow="3375" windowWidth="13545" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -572,7 +572,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -882,6 +882,9 @@
       <c r="D18">
         <v>1</v>
       </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -908,6 +911,9 @@
         <v>375</v>
       </c>
       <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
         <v>1</v>
       </c>
     </row>

</xml_diff>